<commit_message>
changed copy from json to copy library based copies
</commit_message>
<xml_diff>
--- a/output/Deposits Data Lite_recreated.xlsx
+++ b/output/Deposits Data Lite_recreated.xlsx
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,14 +29,11 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,10 +53,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -76,16 +82,16 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>

</xml_diff>